<commit_message>
data base tools altered
</commit_message>
<xml_diff>
--- a/1.xlsx
+++ b/1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/melmav/Documents/pycoders/home_library/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DanilMelnikov\Documents\GitHub\home_library\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4851BB68-FDFB-AE4D-9576-747E70BF79BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE1190BD-288E-4CB5-AFF6-667D73D4D3C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2384,21 +2384,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:I244"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="150" workbookViewId="0">
       <selection activeCell="I249" sqref="I249"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="21.1640625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="50.5" customWidth="1"/>
-    <col min="5" max="5" width="28.83203125" customWidth="1"/>
+    <col min="3" max="3" width="21.1796875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="50.453125" customWidth="1"/>
+    <col min="5" max="5" width="28.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2424,7 +2423,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2450,7 +2449,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2476,7 +2475,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -2502,7 +2501,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -2528,7 +2527,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -2551,7 +2550,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -2577,7 +2576,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -2600,7 +2599,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -2623,7 +2622,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -2649,7 +2648,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -2672,7 +2671,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -2698,7 +2697,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -2721,7 +2720,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -2744,7 +2743,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -2767,7 +2766,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -2790,7 +2789,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -2813,7 +2812,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -2836,7 +2835,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -2862,7 +2861,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -2885,7 +2884,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -2908,7 +2907,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -2931,7 +2930,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -2954,7 +2953,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -2980,7 +2979,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -3003,7 +3002,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>38</v>
       </c>
@@ -3026,7 +3025,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>38</v>
       </c>
@@ -3049,7 +3048,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>38</v>
       </c>
@@ -3069,7 +3068,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
         <v>38</v>
       </c>
@@ -3092,7 +3091,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
         <v>38</v>
       </c>
@@ -3112,7 +3111,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>38</v>
       </c>
@@ -3129,7 +3128,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>38</v>
       </c>
@@ -3155,7 +3154,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="33" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
         <v>38</v>
       </c>
@@ -3178,7 +3177,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="34" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
         <v>38</v>
       </c>
@@ -3201,7 +3200,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="35" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
         <v>38</v>
       </c>
@@ -3224,7 +3223,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="36" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
         <v>38</v>
       </c>
@@ -3247,7 +3246,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="37" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B37" t="s">
         <v>38</v>
       </c>
@@ -3270,7 +3269,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="38" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
         <v>38</v>
       </c>
@@ -3293,7 +3292,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="39" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B39" t="s">
         <v>38</v>
       </c>
@@ -3313,7 +3312,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="40" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B40" t="s">
         <v>38</v>
       </c>
@@ -3336,7 +3335,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="41" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B41" t="s">
         <v>38</v>
       </c>
@@ -3356,7 +3355,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="42" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B42" t="s">
         <v>38</v>
       </c>
@@ -3376,7 +3375,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="43" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B43" t="s">
         <v>38</v>
       </c>
@@ -3399,7 +3398,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="44" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B44" t="s">
         <v>38</v>
       </c>
@@ -3422,7 +3421,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="45" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B45" t="s">
         <v>38</v>
       </c>
@@ -3442,7 +3441,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="46" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
         <v>38</v>
       </c>
@@ -3465,7 +3464,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="47" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B47" t="s">
         <v>38</v>
       </c>
@@ -3488,7 +3487,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="48" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B48" t="s">
         <v>38</v>
       </c>
@@ -3508,7 +3507,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="49" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B49" t="s">
         <v>38</v>
       </c>
@@ -3531,7 +3530,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="50" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B50" t="s">
         <v>38</v>
       </c>
@@ -3554,7 +3553,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="51" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B51" t="s">
         <v>38</v>
       </c>
@@ -3577,7 +3576,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="52" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B52" t="s">
         <v>127</v>
       </c>
@@ -3597,7 +3596,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B53" t="s">
         <v>127</v>
       </c>
@@ -3617,7 +3616,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="54" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B54" t="s">
         <v>127</v>
       </c>
@@ -3637,7 +3636,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="55" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B55" t="s">
         <v>127</v>
       </c>
@@ -3657,7 +3656,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B56" t="s">
         <v>127</v>
       </c>
@@ -3680,7 +3679,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="57" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B57" t="s">
         <v>127</v>
       </c>
@@ -3700,7 +3699,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="58" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B58" t="s">
         <v>127</v>
       </c>
@@ -3720,7 +3719,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="59" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B59" t="s">
         <v>127</v>
       </c>
@@ -3740,7 +3739,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="60" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B60" t="s">
         <v>127</v>
       </c>
@@ -3760,7 +3759,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="61" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B61" t="s">
         <v>127</v>
       </c>
@@ -3780,7 +3779,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="62" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B62" t="s">
         <v>127</v>
       </c>
@@ -3800,7 +3799,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="63" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B63" t="s">
         <v>127</v>
       </c>
@@ -3820,7 +3819,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="64" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B64" t="s">
         <v>127</v>
       </c>
@@ -3840,7 +3839,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="65" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B65" t="s">
         <v>127</v>
       </c>
@@ -3860,7 +3859,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="66" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B66" t="s">
         <v>127</v>
       </c>
@@ -3880,7 +3879,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="67" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B67" t="s">
         <v>127</v>
       </c>
@@ -3900,7 +3899,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="68" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B68" t="s">
         <v>127</v>
       </c>
@@ -3920,7 +3919,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="69" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B69" t="s">
         <v>127</v>
       </c>
@@ -3940,7 +3939,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="70" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B70" t="s">
         <v>127</v>
       </c>
@@ -3960,7 +3959,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="71" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B71" t="s">
         <v>127</v>
       </c>
@@ -3980,7 +3979,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="72" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B72" t="s">
         <v>127</v>
       </c>
@@ -4000,7 +3999,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="73" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B73" t="s">
         <v>127</v>
       </c>
@@ -4020,7 +4019,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="74" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B74" t="s">
         <v>127</v>
       </c>
@@ -4040,7 +4039,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="75" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B75" t="s">
         <v>127</v>
       </c>
@@ -4060,7 +4059,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="76" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B76" t="s">
         <v>127</v>
       </c>
@@ -4080,7 +4079,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="77" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B77" t="s">
         <v>201</v>
       </c>
@@ -4100,7 +4099,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="78" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B78" t="s">
         <v>201</v>
       </c>
@@ -4120,7 +4119,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="79" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B79" t="s">
         <v>201</v>
       </c>
@@ -4140,7 +4139,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="80" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B80" t="s">
         <v>201</v>
       </c>
@@ -4160,7 +4159,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="81" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B81" t="s">
         <v>201</v>
       </c>
@@ -4180,7 +4179,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="82" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B82" t="s">
         <v>201</v>
       </c>
@@ -4203,7 +4202,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="83" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B83" t="s">
         <v>201</v>
       </c>
@@ -4223,7 +4222,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="84" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B84" t="s">
         <v>201</v>
       </c>
@@ -4240,7 +4239,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="85" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B85" t="s">
         <v>201</v>
       </c>
@@ -4260,7 +4259,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="86" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B86" t="s">
         <v>201</v>
       </c>
@@ -4277,7 +4276,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="87" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B87" t="s">
         <v>201</v>
       </c>
@@ -4294,7 +4293,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="88" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B88" t="s">
         <v>201</v>
       </c>
@@ -4317,7 +4316,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="89" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B89" t="s">
         <v>201</v>
       </c>
@@ -4337,7 +4336,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="90" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B90" t="s">
         <v>201</v>
       </c>
@@ -4357,7 +4356,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="91" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B91" t="s">
         <v>201</v>
       </c>
@@ -4377,7 +4376,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="92" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B92" t="s">
         <v>201</v>
       </c>
@@ -4400,7 +4399,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="93" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B93" t="s">
         <v>201</v>
       </c>
@@ -4423,7 +4422,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="94" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B94" t="s">
         <v>201</v>
       </c>
@@ -4446,7 +4445,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="95" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B95" t="s">
         <v>201</v>
       </c>
@@ -4469,7 +4468,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="96" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B96" t="s">
         <v>201</v>
       </c>
@@ -4492,7 +4491,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="97" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B97" t="s">
         <v>201</v>
       </c>
@@ -4512,7 +4511,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="98" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B98" t="s">
         <v>201</v>
       </c>
@@ -4535,7 +4534,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="99" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B99" t="s">
         <v>201</v>
       </c>
@@ -4558,7 +4557,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="100" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B100" t="s">
         <v>201</v>
       </c>
@@ -4581,7 +4580,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="101" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B101" t="s">
         <v>270</v>
       </c>
@@ -4604,7 +4603,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="102" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B102" t="s">
         <v>270</v>
       </c>
@@ -4627,7 +4626,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="103" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B103" t="s">
         <v>270</v>
       </c>
@@ -4650,7 +4649,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="104" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B104" t="s">
         <v>270</v>
       </c>
@@ -4673,7 +4672,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="105" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B105" t="s">
         <v>270</v>
       </c>
@@ -4696,7 +4695,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="106" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B106" t="s">
         <v>270</v>
       </c>
@@ -4719,7 +4718,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="107" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B107" t="s">
         <v>270</v>
       </c>
@@ -4745,7 +4744,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="108" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B108" t="s">
         <v>270</v>
       </c>
@@ -4768,7 +4767,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="109" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B109" t="s">
         <v>270</v>
       </c>
@@ -4791,7 +4790,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="110" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B110" t="s">
         <v>270</v>
       </c>
@@ -4814,7 +4813,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="111" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B111" t="s">
         <v>270</v>
       </c>
@@ -4837,7 +4836,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="112" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B112" t="s">
         <v>270</v>
       </c>
@@ -4857,7 +4856,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="113" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B113" t="s">
         <v>270</v>
       </c>
@@ -4883,7 +4882,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="114" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B114" t="s">
         <v>270</v>
       </c>
@@ -4906,7 +4905,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="115" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B115" t="s">
         <v>270</v>
       </c>
@@ -4926,7 +4925,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="116" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B116" t="s">
         <v>270</v>
       </c>
@@ -4949,7 +4948,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="117" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B117" t="s">
         <v>270</v>
       </c>
@@ -4972,7 +4971,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="118" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B118" t="s">
         <v>270</v>
       </c>
@@ -4995,7 +4994,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="119" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B119" t="s">
         <v>270</v>
       </c>
@@ -5015,7 +5014,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="120" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B120" t="s">
         <v>270</v>
       </c>
@@ -5035,7 +5034,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="121" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="121" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B121" t="s">
         <v>331</v>
       </c>
@@ -5055,7 +5054,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="122" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B122" t="s">
         <v>331</v>
       </c>
@@ -5075,7 +5074,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="123" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B123" t="s">
         <v>331</v>
       </c>
@@ -5095,7 +5094,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="124" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B124" t="s">
         <v>331</v>
       </c>
@@ -5115,7 +5114,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="125" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B125" t="s">
         <v>331</v>
       </c>
@@ -5138,7 +5137,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="126" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B126" t="s">
         <v>331</v>
       </c>
@@ -5158,7 +5157,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="127" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B127" t="s">
         <v>331</v>
       </c>
@@ -5178,7 +5177,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="128" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B128" t="s">
         <v>331</v>
       </c>
@@ -5198,7 +5197,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="129" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="129" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B129" t="s">
         <v>331</v>
       </c>
@@ -5218,7 +5217,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="130" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="130" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B130" t="s">
         <v>331</v>
       </c>
@@ -5238,7 +5237,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="131" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B131" t="s">
         <v>331</v>
       </c>
@@ -5261,7 +5260,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="132" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="132" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B132" t="s">
         <v>331</v>
       </c>
@@ -5284,7 +5283,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="133" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B133" t="s">
         <v>331</v>
       </c>
@@ -5304,7 +5303,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="134" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B134" t="s">
         <v>331</v>
       </c>
@@ -5324,7 +5323,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="135" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B135" t="s">
         <v>331</v>
       </c>
@@ -5344,7 +5343,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="136" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B136" t="s">
         <v>331</v>
       </c>
@@ -5364,7 +5363,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="137" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B137" t="s">
         <v>331</v>
       </c>
@@ -5384,7 +5383,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="138" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B138" t="s">
         <v>331</v>
       </c>
@@ -5404,7 +5403,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="139" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B139" t="s">
         <v>331</v>
       </c>
@@ -5424,7 +5423,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="140" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B140" t="s">
         <v>331</v>
       </c>
@@ -5447,7 +5446,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="141" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B141" t="s">
         <v>331</v>
       </c>
@@ -5467,7 +5466,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="142" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B142" t="s">
         <v>331</v>
       </c>
@@ -5487,7 +5486,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="143" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B143" t="s">
         <v>331</v>
       </c>
@@ -5507,7 +5506,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="144" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B144" t="s">
         <v>331</v>
       </c>
@@ -5530,7 +5529,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="145" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B145" t="s">
         <v>331</v>
       </c>
@@ -5550,7 +5549,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="146" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B146" t="s">
         <v>331</v>
       </c>
@@ -5570,7 +5569,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="147" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B147" t="s">
         <v>331</v>
       </c>
@@ -5590,7 +5589,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="148" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B148" t="s">
         <v>411</v>
       </c>
@@ -5610,7 +5609,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="149" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B149" t="s">
         <v>411</v>
       </c>
@@ -5630,7 +5629,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="150" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B150" t="s">
         <v>411</v>
       </c>
@@ -5650,7 +5649,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="151" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B151" t="s">
         <v>411</v>
       </c>
@@ -5670,7 +5669,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="152" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B152" t="s">
         <v>411</v>
       </c>
@@ -5690,7 +5689,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="153" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B153" t="s">
         <v>411</v>
       </c>
@@ -5713,7 +5712,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="154" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B154" t="s">
         <v>411</v>
       </c>
@@ -5733,7 +5732,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="155" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B155" t="s">
         <v>411</v>
       </c>
@@ -5753,7 +5752,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="156" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B156" t="s">
         <v>411</v>
       </c>
@@ -5773,7 +5772,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="157" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B157" t="s">
         <v>411</v>
       </c>
@@ -5793,7 +5792,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="158" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B158" t="s">
         <v>411</v>
       </c>
@@ -5813,7 +5812,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="159" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B159" t="s">
         <v>411</v>
       </c>
@@ -5830,7 +5829,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="160" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B160" t="s">
         <v>411</v>
       </c>
@@ -5850,7 +5849,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="161" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B161" t="s">
         <v>411</v>
       </c>
@@ -5870,7 +5869,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="162" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B162" t="s">
         <v>411</v>
       </c>
@@ -5890,7 +5889,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="163" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B163" t="s">
         <v>411</v>
       </c>
@@ -5907,7 +5906,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="164" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B164" t="s">
         <v>411</v>
       </c>
@@ -5927,7 +5926,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="165" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B165" t="s">
         <v>411</v>
       </c>
@@ -5947,7 +5946,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="166" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B166" t="s">
         <v>411</v>
       </c>
@@ -5967,7 +5966,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="167" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B167" t="s">
         <v>411</v>
       </c>
@@ -5987,7 +5986,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="168" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B168" t="s">
         <v>411</v>
       </c>
@@ -6007,7 +6006,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="169" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B169" t="s">
         <v>411</v>
       </c>
@@ -6027,7 +6026,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="170" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B170" t="s">
         <v>411</v>
       </c>
@@ -6047,7 +6046,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="171" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B171" t="s">
         <v>411</v>
       </c>
@@ -6067,7 +6066,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="172" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B172" t="s">
         <v>411</v>
       </c>
@@ -6087,7 +6086,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="173" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B173" t="s">
         <v>468</v>
       </c>
@@ -6107,7 +6106,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="174" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B174" t="s">
         <v>468</v>
       </c>
@@ -6127,7 +6126,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="175" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B175" t="s">
         <v>468</v>
       </c>
@@ -6147,7 +6146,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="176" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B176" t="s">
         <v>468</v>
       </c>
@@ -6167,7 +6166,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="177" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B177" t="s">
         <v>468</v>
       </c>
@@ -6187,7 +6186,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="178" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="178" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B178" t="s">
         <v>468</v>
       </c>
@@ -6207,7 +6206,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="179" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="179" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B179" t="s">
         <v>468</v>
       </c>
@@ -6227,7 +6226,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="180" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="180" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B180" t="s">
         <v>468</v>
       </c>
@@ -6247,7 +6246,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="181" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="181" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B181" t="s">
         <v>468</v>
       </c>
@@ -6267,7 +6266,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="182" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B182" t="s">
         <v>468</v>
       </c>
@@ -6287,7 +6286,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="183" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B183" t="s">
         <v>468</v>
       </c>
@@ -6307,7 +6306,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="184" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B184" t="s">
         <v>468</v>
       </c>
@@ -6327,7 +6326,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="185" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B185" t="s">
         <v>468</v>
       </c>
@@ -6347,7 +6346,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="186" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B186" t="s">
         <v>468</v>
       </c>
@@ -6367,7 +6366,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="187" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="187" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B187" t="s">
         <v>468</v>
       </c>
@@ -6387,7 +6386,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="188" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B188" t="s">
         <v>468</v>
       </c>
@@ -6407,7 +6406,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="189" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B189" t="s">
         <v>468</v>
       </c>
@@ -6427,7 +6426,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="190" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B190" t="s">
         <v>468</v>
       </c>
@@ -6447,7 +6446,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="191" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="191" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B191" t="s">
         <v>468</v>
       </c>
@@ -6467,7 +6466,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="192" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B192" t="s">
         <v>468</v>
       </c>
@@ -6487,7 +6486,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="193" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="193" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B193" t="s">
         <v>468</v>
       </c>
@@ -6507,7 +6506,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="194" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="194" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B194" t="s">
         <v>468</v>
       </c>
@@ -6527,7 +6526,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="195" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="195" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B195" t="s">
         <v>519</v>
       </c>
@@ -6547,7 +6546,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="196" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="196" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B196" t="s">
         <v>519</v>
       </c>
@@ -6567,7 +6566,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="197" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="197" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B197" t="s">
         <v>519</v>
       </c>
@@ -6590,7 +6589,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="198" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="198" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B198" t="s">
         <v>519</v>
       </c>
@@ -6613,7 +6612,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="199" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="199" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B199" t="s">
         <v>519</v>
       </c>
@@ -6636,7 +6635,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="200" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="200" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B200" t="s">
         <v>519</v>
       </c>
@@ -6656,7 +6655,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="201" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="201" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B201" t="s">
         <v>519</v>
       </c>
@@ -6676,7 +6675,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="202" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="202" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B202" t="s">
         <v>519</v>
       </c>
@@ -6696,7 +6695,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="203" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="203" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B203" t="s">
         <v>519</v>
       </c>
@@ -6716,7 +6715,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="204" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="204" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B204" t="s">
         <v>519</v>
       </c>
@@ -6736,7 +6735,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="205" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="205" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B205" t="s">
         <v>519</v>
       </c>
@@ -6756,7 +6755,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="206" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="206" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B206" t="s">
         <v>519</v>
       </c>
@@ -6776,7 +6775,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="207" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="207" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B207" t="s">
         <v>519</v>
       </c>
@@ -6796,7 +6795,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="208" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="208" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B208" t="s">
         <v>519</v>
       </c>
@@ -6816,7 +6815,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="209" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="209" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B209" t="s">
         <v>519</v>
       </c>
@@ -6836,7 +6835,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="210" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="210" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B210" t="s">
         <v>519</v>
       </c>
@@ -6856,7 +6855,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="211" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="211" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B211" t="s">
         <v>519</v>
       </c>
@@ -6876,7 +6875,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="212" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="212" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B212" t="s">
         <v>519</v>
       </c>
@@ -6896,7 +6895,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="213" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="213" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B213" t="s">
         <v>519</v>
       </c>
@@ -6916,7 +6915,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="214" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="214" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B214" t="s">
         <v>519</v>
       </c>
@@ -6936,7 +6935,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="215" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="215" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B215" t="s">
         <v>519</v>
       </c>
@@ -6956,7 +6955,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="216" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="216" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B216" t="s">
         <v>519</v>
       </c>
@@ -6976,7 +6975,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="217" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="217" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B217" t="s">
         <v>519</v>
       </c>
@@ -6996,7 +6995,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="218" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="218" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B218" t="s">
         <v>519</v>
       </c>
@@ -7013,7 +7012,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="219" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="219" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B219" t="s">
         <v>519</v>
       </c>
@@ -7033,7 +7032,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="220" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="220" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B220" t="s">
         <v>519</v>
       </c>
@@ -7053,7 +7052,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="221" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="221" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B221" t="s">
         <v>519</v>
       </c>
@@ -7073,7 +7072,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="222" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="222" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B222" t="s">
         <v>519</v>
       </c>
@@ -7093,7 +7092,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="223" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="223" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B223" t="s">
         <v>519</v>
       </c>
@@ -7113,7 +7112,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="224" spans="2:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="224" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B224" t="s">
         <v>519</v>
       </c>
@@ -7133,7 +7132,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="225" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="225" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B225" t="s">
         <v>519</v>
       </c>
@@ -7153,7 +7152,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="226" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="226" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B226" t="s">
         <v>519</v>
       </c>
@@ -7176,7 +7175,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="227" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="227" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B227" t="s">
         <v>615</v>
       </c>
@@ -7196,7 +7195,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="228" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="228" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B228" t="s">
         <v>615</v>
       </c>
@@ -7213,7 +7212,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="229" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="229" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B229" t="s">
         <v>615</v>
       </c>
@@ -7233,7 +7232,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="230" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="230" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B230" t="s">
         <v>615</v>
       </c>
@@ -7250,7 +7249,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="231" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="231" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B231" t="s">
         <v>615</v>
       </c>
@@ -7273,7 +7272,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="232" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="232" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B232" t="s">
         <v>615</v>
       </c>
@@ -7293,7 +7292,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="233" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="233" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B233" t="s">
         <v>615</v>
       </c>
@@ -7313,7 +7312,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="234" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="234" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B234" t="s">
         <v>615</v>
       </c>
@@ -7330,7 +7329,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="235" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="235" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B235" t="s">
         <v>615</v>
       </c>
@@ -7347,7 +7346,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="236" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="236" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B236" t="s">
         <v>615</v>
       </c>
@@ -7367,7 +7366,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="237" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="237" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B237" t="s">
         <v>615</v>
       </c>
@@ -7387,7 +7386,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="238" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="238" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B238" t="s">
         <v>615</v>
       </c>
@@ -7407,7 +7406,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="239" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="239" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B239" t="s">
         <v>615</v>
       </c>
@@ -7424,7 +7423,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="240" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="240" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B240" t="s">
         <v>615</v>
       </c>
@@ -7444,7 +7443,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="241" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="241" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B241" t="s">
         <v>615</v>
       </c>
@@ -7464,7 +7463,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="242" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="242" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B242" t="s">
         <v>615</v>
       </c>
@@ -7481,7 +7480,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="243" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="243" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B243" t="s">
         <v>615</v>
       </c>
@@ -7501,7 +7500,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="244" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="244" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B244">
         <v>3</v>
       </c>
@@ -7519,23 +7518,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H244" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="Animals - 25 Tiere zeichnen mit Watercolor-Effekt - Mit Vorlagen zum Abpausen"/>
-        <filter val="Die Zuckermeister (1). Der magische Pakt"/>
-        <filter val="Einfach nachhaltig kochen - Der Umwelt zuliebe - Plastikfrei einkaufen, vegetarisch kochen und die Erde ein kleines bisschen besser machen - Tipps für mehr Nachhaltigkeit im Alltag, Zero-Waste-Einkaufsratgeber und mehr"/>
-        <filter val="Häkeln im Makramee-Style - Die angesagte Trend-Optik nun auch zum Häkeln"/>
-        <filter val="Natur in Pastell - Tiere, Blumen Landschaften: Vom ersten Schritt zum schönen Bild"/>
-        <filter val="Pernilla oder Wie die Beatles meine viel zu große Familie retteten"/>
-        <filter val="Unser Zuhause - Eine Wimmelbilder-Geschichte. Vierfarbiges Pappbilderbuch"/>
-        <filter val="Van Life Kitchen - Die Abenteuer-Outdoor-Küche - Über 60 Rezepte zum Camping, Wandern und mehr"/>
-        <filter val="Voll gemütlich. Das Kinder Künstlerbuch vom Wohnen und Bauen - Mit Schutzumschlag zum"/>
-        <filter val="Watercolor Porträt - 20 berühmte Persönlichkeiten Step-by-Step zeichnen und mit Aquarell kolorieren - Mit praktischen Vorlagen zum Abpausen"/>
-        <filter val="Zusammen!"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:H244" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>